<commit_message>
FEATURE/Ajout 00 - JDD GENERATOR et my.JDDGenerator
</commit_message>
<xml_diff>
--- a/TNR/TrameJDD.xlsx
+++ b/TNR/TrameJDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="1"/>
+    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -110,9 +110,13 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> instead of the value of the mentioned field name.</t>
     </r>
+  </si>
+  <si>
+    <t>Champ</t>
   </si>
 </sst>
 </file>
@@ -222,6 +226,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -234,6 +239,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1773,7 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E880"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2717,13 +2723,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2731,92 +2737,70 @@
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="17"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="13.2">
+      <c r="B1" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.2">
       <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="13.2">
+    </row>
+    <row r="3" spans="1:2" ht="13.2">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" ht="13.2">
+    </row>
+    <row r="4" spans="1:2" ht="13.2">
       <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="13.2">
+    </row>
+    <row r="5" spans="1:2" ht="13.2">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1">
+    </row>
+    <row r="6" spans="1:2" ht="14.4" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="14"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="14"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="14"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1">
       <c r="A16" s="14"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
feat(JDDGenerator) Ajouter le type dans l'onglet Info de JDD et standardisation du msg addInfoVersion
- pour les varchar type(taille) : varchar (50)
- pour les T_BOOLEAN mettre boolean
- pour les numeric mettre numeric
- mettre les PK en rouge gras
</commit_message>
<xml_diff>
--- a/TNR/TrameJDD.xlsx
+++ b/TNR/TrameJDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="1"/>
+    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>Champ</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PK en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>rouge</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -617,15 +635,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1" collapsed="1"/>
     <col min="6" max="26" width="10.6640625" customWidth="1" collapsed="1"/>
@@ -1634,75 +1653,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z880"/>
+  <dimension ref="A1:AA880"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="26" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="27" width="10.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1">
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="12.75" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="5" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="6" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="7" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="8" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="11" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="12" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="13" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="15" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="16" spans="1:6" ht="12.75" customHeight="1"/>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1"/>
     <row r="19" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
FEAT(JDD.makeTO) Gestion standardisé des TAB
-Ajout gestion $TAB$nom et $TABSELECTED$nom dans LOCATOR IHMTO des JDD
-Ajout des noms TA B et TABSELECTED dans JDD.GLOBAL
+Correction erreur dans InfoBDD  getDATA_TYPE
</commit_message>
<xml_diff>
--- a/TNR/TrameJDD.xlsx
+++ b/TNR/TrameJDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872"/>
+    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -2638,7 +2638,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -2648,6 +2648,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="19" customFormat="1" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
FEAT (infoBDD) sortir PARA de InfoBDD et corrections diverses
-créer une nouvelle class infoPARA
-créer un nouveau TC pour lancer le remplissage de InfoPARA --> il sera
à lancer après le CHECK PREREQUIS
-inclure tous les champs du JDD y compris les champs NON IHM, ne plus
s'occuper du nombre d'utilisation
-XLS corrections
-JDDGenerator corrections
</commit_message>
<xml_diff>
--- a/TNR/TrameJDD.xlsx
+++ b/TNR/TrameJDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="3"/>
+    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -2638,7 +2638,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>

</xml_diff>

<commit_message>
update TAG GLOBAL mot clé dyn
Renommage des TAG pour REC
button_Valider et button_Supprimer dans GLOBAL --> maj des TC CRE MAJ
SUP de FOU et ZZ TEMPLATE (ACT garde le spécifique car pas le mm ID)
a_Resultat_ID dans GLOBAL --> maj des TC CRE et MAJ  de FOU ACT+ACT.FON
et ZZ TEMPLATE 
input_Filtre_Grille dans GLOBAL --> créer mot clé FILTREGRILLE -->
modifier REC
nbrecordsGRID dans GLOBAL --> modifier REC
td_Grille dans GLOBAL --> créer mot clé dynamique TDGRILLE
Ajout le $NU dans les docs JDD Lisez moi et ORGANISATION DES JDD DE
REFERENCE POUR TNR
</commit_message>
<xml_diff>
--- a/TNR/TrameJDD.xlsx
+++ b/TNR/TrameJDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872"/>
+    <workbookView xWindow="-828" yWindow="348" windowWidth="5064" windowHeight="7872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -127,16 +127,56 @@
       <t>rouge</t>
     </r>
   </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>a_Fournisseur</t>
+  </si>
+  <si>
+    <t>$TAB$ID_CODFOU</t>
+  </si>
+  <si>
+    <t>a_FournisseurSelected</t>
+  </si>
+  <si>
+    <t>$TABSELECTED$ID_CODFOU</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>input_Filtre_Grille</t>
+  </si>
+  <si>
+    <t>td_Grille</t>
+  </si>
+  <si>
+    <t>$FILTREGRILLE$ID_CODFOU</t>
+  </si>
+  <si>
+    <t>EXEMPLES</t>
+  </si>
+  <si>
+    <t>$TDGRILLE$ID_CODFOU</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,8 +296,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +375,12 @@
         <bgColor rgb="FFA7E3B7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -356,79 +413,112 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="11" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="21" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="21" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="21" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="21" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="24">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="20"/>
+    <cellStyle name="Normal 11" xfId="21"/>
+    <cellStyle name="Normal 12" xfId="11"/>
+    <cellStyle name="Normal 13" xfId="13"/>
+    <cellStyle name="Normal 14" xfId="23"/>
+    <cellStyle name="Normal 15" xfId="22"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 2 2" xfId="6"/>
+    <cellStyle name="Normal 2 2 2" xfId="15"/>
+    <cellStyle name="Normal 2 3" xfId="12"/>
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 3 2 2" xfId="16"/>
     <cellStyle name="Normal 4" xfId="1"/>
     <cellStyle name="Normal 5" xfId="4"/>
     <cellStyle name="Normal 6" xfId="5"/>
+    <cellStyle name="Normal 6 2" xfId="14"/>
     <cellStyle name="Normal 7" xfId="8"/>
+    <cellStyle name="Normal 7 2" xfId="17"/>
     <cellStyle name="Normal 8" xfId="9"/>
+    <cellStyle name="Normal 8 2" xfId="18"/>
     <cellStyle name="Normal 9" xfId="10"/>
+    <cellStyle name="Normal 9 2" xfId="19"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -635,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z976"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -2602,15 +2692,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="86.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2623,6 +2714,55 @@
       </c>
       <c r="C1" s="18" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>